<commit_message>
maps worked, added time panel
</commit_message>
<xml_diff>
--- a/GeoList.xlsx
+++ b/GeoList.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/onat/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/onat/Documents/ornament_symmgroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="680" windowWidth="28560" windowHeight="17380" tabRatio="500"/>
+    <workbookView xWindow="1260" yWindow="2460" windowWidth="28560" windowHeight="17380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Geographic" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
   <si>
     <t>Moslem Arab</t>
   </si>
@@ -44,250 +44,253 @@
     <t>Venice</t>
   </si>
   <si>
-    <t>Birgi</t>
-  </si>
-  <si>
-    <t>Akhan</t>
+    <t>Birgi, Turkey</t>
+  </si>
+  <si>
+    <t>Istanbul</t>
+  </si>
+  <si>
+    <t>Akhan, Turkey</t>
   </si>
   <si>
     <t>e</t>
   </si>
   <si>
-    <t>Egridir</t>
-  </si>
-  <si>
-    <t>Incir han</t>
-  </si>
-  <si>
-    <t>Evdir Han</t>
-  </si>
-  <si>
-    <t>Susuz Han</t>
-  </si>
-  <si>
-    <t>Antalya</t>
-  </si>
-  <si>
-    <t>Atabey</t>
-  </si>
-  <si>
-    <t>Boyalikoy</t>
-  </si>
-  <si>
-    <t>Cay</t>
-  </si>
-  <si>
-    <t>Afyon</t>
-  </si>
-  <si>
-    <t>Aksehir</t>
-  </si>
-  <si>
-    <t>Seyitgazi</t>
-  </si>
-  <si>
-    <t>Sivrihisar</t>
-  </si>
-  <si>
-    <t>Ankara</t>
-  </si>
-  <si>
-    <t>Kubadabad</t>
-  </si>
-  <si>
-    <t>Aspendos</t>
-  </si>
-  <si>
-    <t>Obakoy</t>
-  </si>
-  <si>
-    <t>Seydisehir</t>
-  </si>
-  <si>
-    <t>Kurucesme han</t>
-  </si>
-  <si>
-    <t>Meram</t>
-  </si>
-  <si>
-    <t>Ilgin</t>
-  </si>
-  <si>
-    <t>ishakli han</t>
-  </si>
-  <si>
-    <t>Obaköy</t>
-  </si>
-  <si>
-    <t>kiziloren han</t>
-  </si>
-  <si>
-    <t>sadeddin han</t>
-  </si>
-  <si>
-    <t>ermenek</t>
-  </si>
-  <si>
-    <t>sultanhan</t>
-  </si>
-  <si>
-    <t>kirsehir</t>
-  </si>
-  <si>
-    <t>gaferyat koy</t>
-  </si>
-  <si>
-    <t>karaman</t>
-  </si>
-  <si>
-    <t>agzikara han</t>
-  </si>
-  <si>
-    <t>nigde</t>
-  </si>
-  <si>
-    <t>sarihan</t>
-  </si>
-  <si>
-    <t>keykubadiye</t>
-  </si>
-  <si>
-    <t>damsa koy</t>
-  </si>
-  <si>
-    <t>misis</t>
-  </si>
-  <si>
-    <t>develi</t>
-  </si>
-  <si>
-    <t>corum</t>
-  </si>
-  <si>
-    <t>alaca</t>
-  </si>
-  <si>
-    <t>kalehisar</t>
-  </si>
-  <si>
-    <t>kasabakoy</t>
-  </si>
-  <si>
-    <t>cankiri</t>
-  </si>
-  <si>
-    <t>konya</t>
-  </si>
-  <si>
-    <t>ayas</t>
-  </si>
-  <si>
-    <t>oba koy</t>
-  </si>
-  <si>
-    <t>alayhan</t>
-  </si>
-  <si>
-    <t>sinop</t>
-  </si>
-  <si>
-    <t>erkilet</t>
-  </si>
-  <si>
-    <t>bunyan</t>
-  </si>
-  <si>
-    <t>karatay-han</t>
-  </si>
-  <si>
-    <t>pazaroren</t>
-  </si>
-  <si>
-    <t>sivas</t>
-  </si>
-  <si>
-    <t>amasya</t>
-  </si>
-  <si>
-    <t>cakilli han</t>
-  </si>
-  <si>
-    <t>niksar</t>
-  </si>
-  <si>
-    <t>tokat</t>
-  </si>
-  <si>
-    <t>divrigi</t>
-  </si>
-  <si>
-    <t>afsin</t>
-  </si>
-  <si>
-    <t>malatya</t>
-  </si>
-  <si>
-    <t>kemah</t>
-  </si>
-  <si>
-    <t>trabzon</t>
-  </si>
-  <si>
-    <t>harput</t>
-  </si>
-  <si>
-    <t>hani</t>
-  </si>
-  <si>
-    <t>silvan</t>
-  </si>
-  <si>
-    <t>diyarbakir</t>
-  </si>
-  <si>
-    <t>hasan</t>
-  </si>
-  <si>
-    <t>tercan</t>
-  </si>
-  <si>
-    <t>bayburt</t>
-  </si>
-  <si>
-    <t>erzurum</t>
-  </si>
-  <si>
-    <t>erzincan</t>
-  </si>
-  <si>
-    <t>mardin</t>
-  </si>
-  <si>
-    <t>kiziltepe</t>
-  </si>
-  <si>
-    <t>siirt</t>
-  </si>
-  <si>
-    <t>ahlat</t>
-  </si>
-  <si>
-    <t>cukur</t>
-  </si>
-  <si>
-    <t>tatvan</t>
-  </si>
-  <si>
-    <t>horosan</t>
-  </si>
-  <si>
-    <t>asagi soylemez koy</t>
-  </si>
-  <si>
-    <t>van</t>
-  </si>
-  <si>
-    <t>ercis</t>
+    <t>Egridir, Turkey</t>
+  </si>
+  <si>
+    <t>Incir han, Turkey</t>
+  </si>
+  <si>
+    <t>Evdir Han, Turkey</t>
+  </si>
+  <si>
+    <t>Susuz Han, Turkey</t>
+  </si>
+  <si>
+    <t>Antalya, Turkey</t>
+  </si>
+  <si>
+    <t>Atabey, Turkey</t>
+  </si>
+  <si>
+    <t>Boyalikoy, Turkey</t>
+  </si>
+  <si>
+    <t>Çay, Turkey</t>
+  </si>
+  <si>
+    <t>Afyon, Turkey</t>
+  </si>
+  <si>
+    <t>Aksehir, Turkey</t>
+  </si>
+  <si>
+    <t>Seyitgazi, Turkey</t>
+  </si>
+  <si>
+    <t>Sivrihisar, Turkey</t>
+  </si>
+  <si>
+    <t>Ankara, Turkey</t>
+  </si>
+  <si>
+    <t>Kubadabad, Turkey</t>
+  </si>
+  <si>
+    <t>Aspendos, Turkey</t>
+  </si>
+  <si>
+    <t>Obakoy, Turkey</t>
+  </si>
+  <si>
+    <t>Seydisehir, Turkey</t>
+  </si>
+  <si>
+    <t>Kurucesme han, Turkey</t>
+  </si>
+  <si>
+    <t>Meram, Turkey</t>
+  </si>
+  <si>
+    <t>Ilgin, Turkey</t>
+  </si>
+  <si>
+    <t>ishakli han, Turkey</t>
+  </si>
+  <si>
+    <t>Obaköy, Turkey</t>
+  </si>
+  <si>
+    <t>kiziloren han, Turkey</t>
+  </si>
+  <si>
+    <t>sadeddin han, Turkey</t>
+  </si>
+  <si>
+    <t>ermenek, Turkey</t>
+  </si>
+  <si>
+    <t>sultanhan, Turkey</t>
+  </si>
+  <si>
+    <t>kirsehir, Turkey</t>
+  </si>
+  <si>
+    <t>gaferyat koy, Turkey</t>
+  </si>
+  <si>
+    <t>karaman, Turkey</t>
+  </si>
+  <si>
+    <t>agzikara han, Turkey</t>
+  </si>
+  <si>
+    <t>nigde, Turkey</t>
+  </si>
+  <si>
+    <t>sarihan, Turkey</t>
+  </si>
+  <si>
+    <t>keykubadiye, Turkey</t>
+  </si>
+  <si>
+    <t>damsa koy, Turkey</t>
+  </si>
+  <si>
+    <t>misis, Turkey</t>
+  </si>
+  <si>
+    <t>develi, Turkey</t>
+  </si>
+  <si>
+    <t>corum, Turkey</t>
+  </si>
+  <si>
+    <t>alaca, Turkey</t>
+  </si>
+  <si>
+    <t>kalehisar, Turkey</t>
+  </si>
+  <si>
+    <t>kasabakoy, Turkey</t>
+  </si>
+  <si>
+    <t>cankiri, Turkey</t>
+  </si>
+  <si>
+    <t>konya, Turkey</t>
+  </si>
+  <si>
+    <t>ayas, Turkey</t>
+  </si>
+  <si>
+    <t>oba koy, Turkey</t>
+  </si>
+  <si>
+    <t>alayhan, Turkey</t>
+  </si>
+  <si>
+    <t>sinop, Turkey</t>
+  </si>
+  <si>
+    <t>erkilet, Turkey</t>
+  </si>
+  <si>
+    <t>bunyan, Turkey</t>
+  </si>
+  <si>
+    <t>karatay han, Turkey</t>
+  </si>
+  <si>
+    <t>pazaroren, Turkey</t>
+  </si>
+  <si>
+    <t>sivas, Turkey</t>
+  </si>
+  <si>
+    <t>amasya, Turkey</t>
+  </si>
+  <si>
+    <t>cakilli han, Turkey</t>
+  </si>
+  <si>
+    <t>niksar, Turkey</t>
+  </si>
+  <si>
+    <t>tokat, Turkey</t>
+  </si>
+  <si>
+    <t>divrigi, Turkey</t>
+  </si>
+  <si>
+    <t>afsin, Turkey</t>
+  </si>
+  <si>
+    <t>malatya, Turkey</t>
+  </si>
+  <si>
+    <t>kemah, Turkey</t>
+  </si>
+  <si>
+    <t>trabzon, Turkey</t>
+  </si>
+  <si>
+    <t>harput, Turkey</t>
+  </si>
+  <si>
+    <t>hani, Turkey</t>
+  </si>
+  <si>
+    <t>silvan, Turkey</t>
+  </si>
+  <si>
+    <t>diyarbakir, Turkey</t>
+  </si>
+  <si>
+    <t>hasan, Turkey</t>
+  </si>
+  <si>
+    <t>tercan, Turkey</t>
+  </si>
+  <si>
+    <t>bayburt, Turkey</t>
+  </si>
+  <si>
+    <t>erzurum, Turkey</t>
+  </si>
+  <si>
+    <t>erzincan, Turkey</t>
+  </si>
+  <si>
+    <t>mardin, Turkey</t>
+  </si>
+  <si>
+    <t>kiziltepe, Turkey</t>
+  </si>
+  <si>
+    <t>siirt, Turkey</t>
+  </si>
+  <si>
+    <t>ahlat, Turkey</t>
+  </si>
+  <si>
+    <t>cukur, Turkey</t>
+  </si>
+  <si>
+    <t>tatvan, Turkey</t>
+  </si>
+  <si>
+    <t>horosan, Turkey</t>
+  </si>
+  <si>
+    <t>asagi soylemez koy, Turkey</t>
+  </si>
+  <si>
+    <t>van, Turkey</t>
+  </si>
+  <si>
+    <t>ercis, Turkey</t>
   </si>
 </sst>
 </file>
@@ -631,426 +634,429 @@
       <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="E3" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E6" s="4" t="s">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E7" s="4" t="s">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E8" s="4" t="s">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E9" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E10" s="4" t="s">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E8" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E11" s="4" t="s">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E9" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E10" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E12" s="4" t="s">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E11" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E13" s="4" t="s">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E12" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E14" s="4" t="s">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E13" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E15" s="4" t="s">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E14" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E16" s="4" t="s">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E15" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E17" s="4" t="s">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E16" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E18" s="4" t="s">
+    <row r="17" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E17" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E19" s="4" t="s">
+    <row r="18" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E18" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E20" s="4" t="s">
+    <row r="19" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E19" s="5" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E20" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E21" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E22" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E23" s="4" t="s">
+    <row r="22" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E22" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E24" s="4" t="s">
+    <row r="23" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E23" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E25" s="4" t="s">
+    <row r="24" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E24" s="5" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E25" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E26" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E27" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E28" s="4" t="s">
+    <row r="27" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E27" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E29" s="4" t="s">
+    <row r="28" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E28" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E30" s="4" t="s">
+    <row r="29" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E29" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E31" s="4" t="s">
+    <row r="30" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E30" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E32" s="4" t="s">
+    <row r="31" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E31" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E33" s="4" t="s">
+    <row r="32" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E32" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E34" s="4" t="s">
+    <row r="33" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E33" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E35" s="4" t="s">
+    <row r="34" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E34" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E36" s="4" t="s">
+    <row r="35" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E35" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E37" s="4" t="s">
+    <row r="36" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E36" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E38" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E39" s="4" t="s">
+    <row r="37" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E37" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E40" s="4" t="s">
+    <row r="38" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E38" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E39" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E41" s="4" t="s">
+    <row r="40" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E40" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E42" s="4" t="s">
+    <row r="41" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E41" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E43" s="4" t="s">
+    <row r="42" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E42" s="5" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E43" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E44" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E45" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E46" s="4" t="s">
+    <row r="45" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E45" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E47" s="4" t="s">
+    <row r="46" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E46" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E48" s="4" t="s">
+    <row r="47" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E47" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E49" s="4" t="s">
+    <row r="48" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E48" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E50" s="4" t="s">
+    <row r="49" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E49" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E51" s="4" t="s">
+    <row r="50" spans="5:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E50" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E52" s="4" t="s">
+    <row r="51" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E51" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E53" s="4" t="s">
+    <row r="52" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E52" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E54" s="4" t="s">
+    <row r="53" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E53" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E55" s="4" t="s">
+    <row r="54" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E54" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E56" s="4" t="s">
+    <row r="55" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E55" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E57" s="4" t="s">
+    <row r="56" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E56" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E58" s="4" t="s">
+    <row r="57" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E57" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E59" s="4" t="s">
+    <row r="58" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E58" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E60" s="4" t="s">
+    <row r="59" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E59" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E61" s="4" t="s">
+    <row r="60" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E60" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E62" s="4" t="s">
+    <row r="61" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E61" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E63" s="4" t="s">
+    <row r="62" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E62" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E64" s="4" t="s">
+    <row r="63" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E63" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E65" s="4" t="s">
+    <row r="64" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E64" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E66" s="4" t="s">
+    <row r="65" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E65" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E67" s="4" t="s">
+    <row r="66" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E66" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E68" s="4" t="s">
+    <row r="67" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E67" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E69" s="4" t="s">
+    <row r="68" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E68" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E70" s="4" t="s">
+    <row r="69" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E69" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E71" s="4" t="s">
+    <row r="70" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E70" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E72" s="4" t="s">
+    <row r="71" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E71" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E73" s="4" t="s">
+    <row r="72" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E72" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E74" s="4" t="s">
+    <row r="73" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E73" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E75" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="76" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E76" s="4" t="s">
+    <row r="74" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E74" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="77" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E77" s="4" t="s">
+    <row r="75" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E75" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E76" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="78" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E78" s="4" t="s">
+    <row r="77" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E77" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="79" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E79" s="4" t="s">
+    <row r="78" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E78" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="80" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E80" s="4" t="s">
+    <row r="79" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E79" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="81" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E81" s="4" t="s">
+    <row r="80" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E80" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="82" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E82" s="4" t="s">
+    <row r="81" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E81" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="83" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E83" s="4" t="s">
+    <row r="82" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E82" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E84" s="4" t="s">
+    <row r="83" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E83" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="5:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="E85" s="4" t="s">
+    <row r="84" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E84" s="5" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E85" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>